<commit_message>
fixed utilis / added evaluing counter
</commit_message>
<xml_diff>
--- a/knapsack_cpp/data/results.xlsx
+++ b/knapsack_cpp/data/results.xlsx
@@ -5,11 +5,11 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pesa/Documents/UNI/of_v0.9.8_osx_release/apps/naturalComp/examples/cpp/knapsack_hard/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pesa/Documents/UNI/natComp/KnapsackDFO/knapsack_cpp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1940" yWindow="40" windowWidth="28160" windowHeight="16820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="640" yWindow="40" windowWidth="28160" windowHeight="16820" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1356" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="649">
   <si>
     <t xml:space="preserve"> problem SENTO1.DAT</t>
   </si>
@@ -1963,6 +1963,18 @@
   </si>
   <si>
     <t>best weight obtained : 9444</t>
+  </si>
+  <si>
+    <t>algo: Swarm's Best, greed/safety ratio: 0.0452734</t>
+  </si>
+  <si>
+    <t>fitness: 2.96191, best fly index: 11, best fly location: 1,0,1,1,1,0,1,0,0,0,1,1,1,1,0,0,0,1,0,0,1,1,1,0,0,1,0,0,1,1,1,0,1,0,0,0,0,0,0,0,1,0,1,0,0,0,0,1,1,1,0,0,0,1,0,0,0,0,1,1,0,0,1,0,0,0,1,0,0,1,1,0,1,1,0,0,0,0,1,0,1,0,0,1,1,1,0,0,0,0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">knap 1: 1360 knap 2: 1445 knap 3: 1410 knap 4: 816 knap 5: 1982 </t>
+  </si>
+  <si>
+    <t>best weight obtained : 9443</t>
   </si>
 </sst>
 </file>
@@ -7773,7 +7785,7 @@
   <dimension ref="A1:AY464"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AM17" sqref="AM17"/>
+      <selection activeCell="AM16" sqref="AM16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8950,7 +8962,7 @@
       <c r="AP16" s="6"/>
       <c r="AQ16" s="6"/>
     </row>
-    <row r="17" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D17" s="14"/>
       <c r="E17" s="7" t="s">
         <v>578</v>
@@ -8965,8 +8977,11 @@
       <c r="Y17" s="14"/>
       <c r="AF17" s="14"/>
       <c r="AG17" s="14"/>
-    </row>
-    <row r="18" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO17" s="7" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="18" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D18" s="14"/>
       <c r="E18" s="8" t="s">
         <v>579</v>
@@ -8982,8 +8997,11 @@
       <c r="Y18" s="14"/>
       <c r="AF18" s="14"/>
       <c r="AG18" s="14"/>
-    </row>
-    <row r="19" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO18" s="8" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="19" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D19" s="14"/>
       <c r="E19" s="8" t="s">
         <v>529</v>
@@ -8999,8 +9017,11 @@
       <c r="Y19" s="14"/>
       <c r="AF19" s="14"/>
       <c r="AG19" s="14"/>
-    </row>
-    <row r="20" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO19" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="20" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D20" s="14"/>
       <c r="E20" s="8" t="s">
         <v>574</v>
@@ -9015,8 +9036,11 @@
       <c r="Y20" s="14"/>
       <c r="AF20" s="14"/>
       <c r="AG20" s="14"/>
-    </row>
-    <row r="21" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO20" s="8" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="21" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D21" s="14"/>
       <c r="E21" s="8" t="s">
         <v>580</v>
@@ -9031,8 +9055,11 @@
       <c r="Y21" s="14"/>
       <c r="AF21" s="14"/>
       <c r="AG21" s="14"/>
-    </row>
-    <row r="22" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO21" s="8" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="22" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D22" s="14"/>
       <c r="E22" s="8" t="s">
         <v>55</v>
@@ -9047,8 +9074,11 @@
       <c r="Y22" s="14"/>
       <c r="AF22" s="14"/>
       <c r="AG22" s="14"/>
-    </row>
-    <row r="23" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO22" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D23" s="14"/>
       <c r="E23" s="8" t="s">
         <v>581</v>
@@ -9063,8 +9093,11 @@
       <c r="Y23" s="14"/>
       <c r="AF23" s="14"/>
       <c r="AG23" s="14"/>
-    </row>
-    <row r="24" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO23" s="8" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="24" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D24" s="14"/>
       <c r="E24" s="8" t="s">
         <v>582</v>
@@ -9079,8 +9112,11 @@
       <c r="Y24" s="14"/>
       <c r="AF24" s="14"/>
       <c r="AG24" s="14"/>
-    </row>
-    <row r="25" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO24" s="8" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="25" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D25" s="14"/>
       <c r="E25" s="8" t="s">
         <v>64</v>
@@ -9095,8 +9131,11 @@
       <c r="Y25" s="14"/>
       <c r="AF25" s="14"/>
       <c r="AG25" s="14"/>
-    </row>
-    <row r="26" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO25" s="8" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="26" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D26" s="14"/>
       <c r="E26" s="5"/>
       <c r="L26" s="8"/>
@@ -9107,8 +9146,9 @@
       <c r="Y26" s="14"/>
       <c r="AF26" s="14"/>
       <c r="AG26" s="14"/>
-    </row>
-    <row r="27" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO26" s="8"/>
+    </row>
+    <row r="27" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D27" s="14"/>
       <c r="E27" s="5"/>
       <c r="L27" s="8"/>
@@ -9119,24 +9159,27 @@
       <c r="Y27" s="14"/>
       <c r="AF27" s="14"/>
       <c r="AG27" s="14"/>
-    </row>
-    <row r="28" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO27" s="8"/>
+    </row>
+    <row r="28" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D28" s="14"/>
       <c r="E28" s="5"/>
       <c r="L28" s="8"/>
       <c r="M28" s="14"/>
       <c r="U28" s="14"/>
       <c r="AG28" s="14"/>
-    </row>
-    <row r="29" spans="4:33" s="10" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AO28" s="8"/>
+    </row>
+    <row r="29" spans="4:41" s="10" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="D29" s="14"/>
       <c r="E29" s="6"/>
       <c r="L29" s="9"/>
       <c r="M29" s="14"/>
       <c r="U29" s="14"/>
       <c r="AG29" s="14"/>
-    </row>
-    <row r="30" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AO29" s="9"/>
+    </row>
+    <row r="30" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D30" s="14"/>
       <c r="E30" s="7" t="s">
         <v>583</v>
@@ -9146,7 +9189,7 @@
       <c r="U30" s="14"/>
       <c r="AG30" s="14"/>
     </row>
-    <row r="31" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D31" s="14"/>
       <c r="E31" s="8" t="s">
         <v>584</v>
@@ -9156,7 +9199,7 @@
       <c r="U31" s="14"/>
       <c r="AG31" s="14"/>
     </row>
-    <row r="32" spans="4:33" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="4:41" s="10" customFormat="1" x14ac:dyDescent="0.2">
       <c r="D32" s="14"/>
       <c r="E32" s="8" t="s">
         <v>309</v>

</xml_diff>